<commit_message>
added class that exports xlsx file to pdf
added class that exports xlsx file to pdf
</commit_message>
<xml_diff>
--- a/1 MALL 2024 Faktura till kattägare (1 katt).xlsx
+++ b/1 MALL 2024 Faktura till kattägare (1 katt).xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Lohaga Kattpensionat</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">Förfallodatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-08-24</t>
   </si>
   <si>
     <t xml:space="preserve">info@lohaga.se</t>
@@ -115,7 +112,7 @@
   <fonts count="12">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -138,7 +135,7 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Monotype Corsiva"/>
       <family val="4"/>
       <charset val="1"/>
@@ -146,14 +143,14 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Monotype Corsiva"/>
       <family val="4"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -161,7 +158,7 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -169,7 +166,7 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -184,7 +181,7 @@
     <font>
       <u val="single"/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -294,11 +291,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,197 +396,25 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office-tema">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="19.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,81 +445,78 @@
       <c r="E6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="F10" s="8" t="n">
-        <f aca="false">SUM(F22)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="12" t="n">
@@ -710,7 +532,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12" t="n">
@@ -733,7 +555,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="14" t="n">
         <f aca="false">F22*0.2</f>
@@ -742,7 +564,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="14" t="n">
         <f aca="false">F22-F20</f>
@@ -751,7 +573,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="8" t="n">
         <f aca="false">SUM(F17:F19)</f>

</xml_diff>

<commit_message>
added ability to read multiple types of cell contents
added ability to read multiple types of cell contents
</commit_message>
<xml_diff>
--- a/1 MALL 2024 Faktura till kattägare (1 katt).xlsx
+++ b/1 MALL 2024 Faktura till kattägare (1 katt).xlsx
@@ -404,10 +404,10 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="19.57"/>
@@ -559,7 +559,7 @@
       </c>
       <c r="F20" s="14" t="n">
         <f aca="false">F22*0.2</f>
-        <v>0</v>
+        <v>246.8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +568,7 @@
       </c>
       <c r="F21" s="14" t="n">
         <f aca="false">F22-F20</f>
-        <v>0</v>
+        <v>987.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,8 +576,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="8" t="n">
-        <f aca="false">SUM(F17:F19)</f>
-        <v>0</v>
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
configured cells to read and dir for deployment
configured cells to read and dir for deployment
</commit_message>
<xml_diff>
--- a/1 MALL 2024 Faktura till kattägare (1 katt).xlsx
+++ b/1 MALL 2024 Faktura till kattägare (1 katt).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">Lohaga Kattpensionat</t>
   </si>
@@ -37,10 +37,16 @@
     <t xml:space="preserve">Fakturadatum</t>
   </si>
   <si>
+    <t xml:space="preserve">2024-10-25</t>
+  </si>
+  <si>
     <t xml:space="preserve">151 50 Enhörna</t>
   </si>
   <si>
     <t xml:space="preserve">Förfallodatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-11-25</t>
   </si>
   <si>
     <t xml:space="preserve">info@lohaga.se</t>
@@ -279,7 +285,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,7 +410,7 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -436,42 +442,46 @@
       <c r="E5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F10" s="8" t="n">
         <v>100</v>
@@ -479,44 +489,44 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="12" t="n">
@@ -532,7 +542,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12" t="n">
@@ -555,7 +565,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F20" s="14" t="n">
         <f aca="false">F22*0.2</f>
@@ -564,7 +574,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F21" s="14" t="n">
         <f aca="false">F22-F20</f>
@@ -573,7 +583,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F22" s="8" t="n">
         <v>1234</v>

</xml_diff>